<commit_message>
agregada funcion de stop
</commit_message>
<xml_diff>
--- a/METODOS.xlsx
+++ b/METODOS.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>DESCRIPCION</t>
   </si>
@@ -129,6 +129,12 @@
   </si>
   <si>
     <t>FUNCION QUE INICIA LA TRANSMISION DE UNO O MAS VALORES HACIA LOS REGISTROS DEL MODULO. SE ESPECIFICA LA DIRECCION MODBUS Y LA CANTIDAD DE REGISTROS A ESCRIBIR. ESTA FUNCION RETORNA VERDADERO SI SE LOGRA INICIAR LA TRANSMISION</t>
+  </si>
+  <si>
+    <t>stop()</t>
+  </si>
+  <si>
+    <t>DETIENE LA COMUNICACION CON EL MODULO</t>
   </si>
 </sst>
 </file>
@@ -181,7 +187,7 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -190,7 +196,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -206,12 +212,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B2:E13" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="B2:E13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="B2:E14" totalsRowShown="0" headerRowDxfId="3">
+  <autoFilter ref="B2:E14"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="METODOS" dataDxfId="3"/>
-    <tableColumn id="2" name="ARGUMENTOS" dataDxfId="2"/>
-    <tableColumn id="3" name="RETORNO" dataDxfId="1"/>
+    <tableColumn id="1" name="METODOS" dataDxfId="2"/>
+    <tableColumn id="2" name="ARGUMENTOS" dataDxfId="1"/>
+    <tableColumn id="3" name="RETORNO" dataDxfId="0"/>
     <tableColumn id="4" name="DESCRIPCION"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight15" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -481,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E13"/>
+  <dimension ref="B2:E14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -668,6 +674,20 @@
         <v>32</v>
       </c>
     </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="3" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>